<commit_message>
Evaluation Files -> Folder round 2 F1-SCORE
</commit_message>
<xml_diff>
--- a/.idea/files/Evaluation/Round2/EvaluationDataset-CEA.xlsx
+++ b/.idea/files/Evaluation/Round2/EvaluationDataset-CEA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ANTHONY\IdeaProjects\STI_Thesis\.idea\files\Evaluation\Round2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94F92218-6D5B-4B54-965D-48A08AF3A640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07113401-F721-489A-8F0D-353B5CC2E436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="1665" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="408">
   <si>
     <t>ResultatDataset1 "0" "1" URI: http://dbpedia.org/resource/Westminster_College_(Missouri)</t>
   </si>
@@ -1253,6 +1253,9 @@
   </si>
   <si>
     <t>ResultatDataset1 "3" "68" URI: 6254</t>
+  </si>
+  <si>
+    <t>F1_Score</t>
   </si>
 </sst>
 </file>
@@ -1614,10 +1617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E278"/>
+  <dimension ref="A1:E279"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A259" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D279" sqref="D279"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6579,6 +6582,15 @@
         <v>1</v>
       </c>
     </row>
+    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A279" t="s">
+        <v>407</v>
+      </c>
+      <c r="B279" s="1">
+        <f>(2*B277*B278)/(B277+B278)</f>
+        <v>0.9850746268656716</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Duplicate fix and New Dataset Round 2
</commit_message>
<xml_diff>
--- a/.idea/files/Evaluation/Round2/EvaluationDataset-CEA.xlsx
+++ b/.idea/files/Evaluation/Round2/EvaluationDataset-CEA.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ANTHONY\IdeaProjects\STI_Thesis\.idea\files\Evaluation\Round2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07113401-F721-489A-8F0D-353B5CC2E436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFE40B4A-2E24-447E-9E38-89EB12EF8C5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="1665" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1620,7 +1620,7 @@
   <dimension ref="A1:E279"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A259" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D279" sqref="D279"/>
+      <selection activeCell="B279" sqref="B279"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>